<commit_message>
Fixed length of table saved in excel sample book
There was a mistake in the initialization of the longest_list_size in the code that prevented it to extract the data to excel sheet when the longest list was in the first location of d2.
</commit_message>
<xml_diff>
--- a/code/results/sample_book.xlsx
+++ b/code/results/sample_book.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -423,45 +423,27 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="n">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B1" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C1" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D1" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="E1" t="n">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F1" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G1" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="H1" t="n">
-        <v>6</v>
-      </c>
-      <c r="I1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J1" t="n">
-        <v>4</v>
-      </c>
-      <c r="K1" t="n">
-        <v>3</v>
-      </c>
-      <c r="L1" t="n">
-        <v>2</v>
-      </c>
-      <c r="M1" t="n">
-        <v>1</v>
-      </c>
-      <c r="N1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -476,7 +458,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -488,25 +470,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="n">
-        <v>3</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
-        <v>4</v>
-      </c>
-      <c r="M2" t="n">
-        <v>1</v>
-      </c>
-      <c r="N2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -520,7 +484,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
@@ -533,24 +497,6 @@
       </c>
       <c r="H3" t="n">
         <v>0</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2</v>
-      </c>
-      <c r="L3" t="n">
-        <v>2</v>
-      </c>
-      <c r="M3" t="n">
-        <v>4</v>
-      </c>
-      <c r="N3" t="n">
-        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -564,7 +510,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
@@ -577,24 +523,6 @@
       </c>
       <c r="H4" t="n">
         <v>0</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -608,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -621,24 +549,6 @@
       </c>
       <c r="H5" t="n">
         <v>0</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" t="n">
-        <v>1</v>
-      </c>
-      <c r="N5" t="n">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>